<commit_message>
Add function to generate annual, el. load profile for non-res buildings based on measured, weekly el. load profiles (#127)
</commit_message>
<xml_diff>
--- a/pycity/inputs/measured_el_loads/Non_res_weekly_el_profiles.xlsx
+++ b/pycity/inputs/measured_el_loads/Non_res_weekly_el_profiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eonakku\home\ebc\jsc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeitsordner_Lokal\PyCharm_workspace\pyCity\pycity\inputs\measured_el_loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39759,8 +39759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I674"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>